<commit_message>
Added a sheet to include an example
</commit_message>
<xml_diff>
--- a/AUF00V00TLXTemplate.xlsx
+++ b/AUF00V00TLXTemplate.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmaa\Documents\GitHub\nasa-tlx_data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6380F96-B7EC-4AFF-AA5A-4B0BFB97BBAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602AC971-44BE-4D88-98F3-BC8E75CCBE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2173" yWindow="2173" windowWidth="19200" windowHeight="11180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
+    <sheet name="Example" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="24">
   <si>
     <t>Stand and alphabet 2 letters</t>
   </si>
@@ -86,7 +87,25 @@
     <t>Directions:</t>
   </si>
   <si>
-    <t>Igonore all headings and align data with cell A1. Place weights directly next to scores. To record weights write the first word in all lower case letters in the correct cell</t>
+    <t>Igonore all headings and align data with cell A1. Place weights directly next to scores. To record weights write the first word in all lower case letters in the correct cell. See example sheet.</t>
+  </si>
+  <si>
+    <t>effort</t>
+  </si>
+  <si>
+    <t>physical</t>
+  </si>
+  <si>
+    <t>mental</t>
+  </si>
+  <si>
+    <t>frustration</t>
+  </si>
+  <si>
+    <t>temporal</t>
+  </si>
+  <si>
+    <t>performance</t>
   </si>
 </sst>
 </file>
@@ -412,17 +431,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1171875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.76171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
@@ -436,7 +455,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -462,7 +481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -476,31 +495,31 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>12</v>
@@ -514,4 +533,274 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63957CC-999A-442D-9E72-56AEA3620384}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A1">
+        <v>45</v>
+      </c>
+      <c r="B1">
+        <v>50</v>
+      </c>
+      <c r="C1">
+        <v>55</v>
+      </c>
+      <c r="D1">
+        <v>50</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>55</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>85</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>65</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>65</v>
+      </c>
+      <c r="C5">
+        <v>70</v>
+      </c>
+      <c r="D5">
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A6">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>